<commit_message>
modify a few more taxonomic names
</commit_message>
<xml_diff>
--- a/data/microbiome_variability_taxa_to_remove-2017-11-03.xlsx
+++ b/data/microbiome_variability_taxa_to_remove-2017-11-03.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="27800" windowHeight="11820"/>
+    <workbookView xWindow="480" yWindow="460" windowWidth="27920" windowHeight="17440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
   <si>
     <t>current_classification</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>Undibacterium oligocarboniphilum</t>
+  </si>
+  <si>
+    <t>Prolinoborus fasciculus</t>
   </si>
 </sst>
 </file>
@@ -669,10 +672,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1015,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E25" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1029,501 +1030,509 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>1549619</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>469</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>202951</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>756892</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>40216756892</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>40214</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>108981</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9">
         <v>202956487316</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>202956</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>70346</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>553384</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>2039240</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>279446</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>41294</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
         <v>59732</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>283</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18">
         <v>225991</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19">
         <v>1194168</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20">
         <v>119416832013</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21">
         <v>470028</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22">
         <v>225971</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23">
         <v>644355</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24">
         <v>1.07400319983744E+16</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25">
         <v>243690</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26">
+        <v>528178</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B27">
         <v>165696</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="1">
-        <v>528178</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B29">
         <v>53406</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B30">
         <v>47878</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B31">
         <v>136843</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B32">
         <v>198620321662</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B33">
         <v>300330</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B34">
         <v>1232139</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B35">
         <v>1392877</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B36">
         <v>23761047885</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B37">
         <v>48736</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B38">
         <v>22</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C38" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B39">
         <v>415996</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B40">
         <v>185950185951</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>46</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B41">
         <v>28213</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B42">
         <v>40323</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B43">
         <v>943830</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B44">
         <v>72763</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B45">
         <v>33057</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C45" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B46">
         <v>666702</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C46" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:C46">
+    <sortCondition ref="A2:A46"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>